<commit_message>
docs: Added Additional Half month allowance.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Demo.xlsx
+++ b/Income And Expenses Forecast Demo.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="135">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -298,7 +298,7 @@
     <t>Entertainment</t>
   </si>
   <si>
-    <t>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</t>
+    <t>Sportify Music Paid For 7th of Each Month.</t>
   </si>
   <si>
     <t>Hair Cutting</t>
@@ -449,6 +449,9 @@
     <t xml:space="preserve">~ Payback $570 to Mom </t>
   </si>
   <si>
+    <t>~ Payback $150.9 to Mom</t>
+  </si>
+  <si>
     <t>~ See the Doctor (Injection) ~ $19
 ~ See the Doctor For Blood Pressure ~ $50
 ~ Brought Lasix 40mg ~ $75
@@ -482,9 +485,6 @@
     <t>~ Payback $800 to Mom</t>
   </si>
   <si>
-    <t>~ Payback $150.9 to Mom (Amazon Books) Hold Till Receive Half Month Allowances</t>
-  </si>
-  <si>
     <t>~ Food And Transport ~ $400</t>
   </si>
   <si>
@@ -510,6 +510,9 @@
   <si>
     <t>- See the Doctor ~ $240
 - Buy Cigarette Buds ~ $800</t>
+  </si>
+  <si>
+    <t>Payback $300 to Mom</t>
   </si>
   <si>
     <t>~ Payback $683 to Mom For Air Ticket.</t>
@@ -4855,7 +4858,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>8688.73</v>
+        <v>9471.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4871,7 +4874,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>8984.36</v>
+        <v>9767.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4887,7 +4890,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -6204,7 +6207,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -6386,7 +6389,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -6466,7 +6469,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -6486,7 +6489,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -6506,7 +6509,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -6582,7 +6585,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -6598,7 +6601,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -6692,7 +6695,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>6792.73</v>
+        <v>7575.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -6861,7 +6864,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -6964,7 +6967,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7387.73</v>
+        <v>8170.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7056,7 +7059,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>7387.73</v>
+        <v>8170.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -7225,7 +7228,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -7240,7 +7243,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -7328,7 +7331,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>8093.73</v>
+        <v>8876.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -7420,7 +7423,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>8093.73</v>
+        <v>8876.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -7589,7 +7592,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -7692,7 +7695,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>8688.73</v>
+        <v>9471.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -8224,7 +8227,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10855.73</v>
+        <v>11638.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8240,7 +8243,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11151.36</v>
+        <v>11934.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -8256,7 +8259,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -9573,7 +9576,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -9755,7 +9758,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -9835,7 +9838,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -9855,7 +9858,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -9875,7 +9878,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -9951,7 +9954,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -9967,7 +9970,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -10061,7 +10064,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>8688.73</v>
+        <v>9471.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -10245,7 +10248,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -10333,7 +10336,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>9554.73</v>
+        <v>10337.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -10425,7 +10428,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>9554.73</v>
+        <v>10337.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -10594,7 +10597,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -10697,7 +10700,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9989.73</v>
+        <v>10772.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -10789,7 +10792,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>9989.73</v>
+        <v>10772.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -10973,7 +10976,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -11061,7 +11064,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10855.73</v>
+        <v>11638.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -11589,7 +11592,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15155.73</v>
+        <v>15938.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -11605,7 +11608,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>15451.36</v>
+        <v>16234.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -11621,7 +11624,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -12942,7 +12945,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>0</v>
@@ -13124,7 +13127,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -13204,7 +13207,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -13224,7 +13227,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -13244,7 +13247,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -13320,7 +13323,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -13336,7 +13339,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -13430,7 +13433,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>10855.73</v>
+        <v>11638.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -13614,7 +13617,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -13702,7 +13705,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12071.73</v>
+        <v>12854.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -13794,7 +13797,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>12071.73</v>
+        <v>12854.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -13963,7 +13966,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -14066,7 +14069,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>13939.73</v>
+        <v>14722.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14158,7 +14161,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>13939.73</v>
+        <v>14722.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -14342,7 +14345,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -14430,7 +14433,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15155.73</v>
+        <v>15938.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -14956,7 +14959,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17051.73</v>
+        <v>17834.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -14972,7 +14975,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>17347.36</v>
+        <v>18130.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14988,7 +14991,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -16305,7 +16308,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -16487,7 +16490,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -16567,7 +16570,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -16587,7 +16590,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -16607,7 +16610,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -16683,7 +16686,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -16699,7 +16702,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -16793,7 +16796,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>15155.73</v>
+        <v>15938.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -16962,7 +16965,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -17065,7 +17068,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>15750.73</v>
+        <v>16533.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17157,7 +17160,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>15750.73</v>
+        <v>16533.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17326,7 +17329,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -17341,7 +17344,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -17429,7 +17432,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>16456.73</v>
+        <v>17239.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -17521,7 +17524,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>16456.73</v>
+        <v>17239.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -17690,7 +17693,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -17793,7 +17796,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17051.73</v>
+        <v>17834.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18326,7 +18329,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19218.73</v>
+        <v>20001.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18342,7 +18345,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19514.36</v>
+        <v>20297.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -18358,7 +18361,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -19675,7 +19678,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -19857,7 +19860,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -19937,7 +19940,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -19957,7 +19960,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -19977,7 +19980,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -20053,7 +20056,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -20069,7 +20072,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -20163,7 +20166,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>17051.73</v>
+        <v>17834.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20347,7 +20350,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -20435,7 +20438,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17917.73</v>
+        <v>18700.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20527,7 +20530,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>17917.73</v>
+        <v>18700.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -20696,7 +20699,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -20799,7 +20802,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>18352.73</v>
+        <v>19135.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -20891,7 +20894,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>18352.73</v>
+        <v>19135.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21075,7 +21078,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -21163,7 +21166,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19218.73</v>
+        <v>20001.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -21689,7 +21692,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>21204.73</v>
+        <v>21987.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -21705,7 +21708,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21500.36</v>
+        <v>22283.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21721,7 +21724,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -23038,7 +23041,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -23220,7 +23223,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -23300,7 +23303,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -23320,7 +23323,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -23340,7 +23343,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -23416,7 +23419,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -23432,7 +23435,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -23526,7 +23529,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>19218.73</v>
+        <v>20001.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23798,7 +23801,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19863.73</v>
+        <v>20646.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -23890,7 +23893,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>19863.73</v>
+        <v>20646.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24059,7 +24062,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -24074,7 +24077,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -24162,7 +24165,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>20569.73</v>
+        <v>21352.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24254,7 +24257,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>20569.73</v>
+        <v>21352.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24423,7 +24426,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -24526,7 +24529,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>21204.73</v>
+        <v>21987.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25058,7 +25061,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>24454.73</v>
+        <v>25237.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25074,7 +25077,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>24750.36</v>
+        <v>25533.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -25090,7 +25093,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -26411,7 +26414,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="37">
         <v>68</v>
@@ -26593,7 +26596,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -26673,7 +26676,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -26693,7 +26696,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -26713,7 +26716,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -26789,7 +26792,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -26805,7 +26808,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -26899,7 +26902,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>21204.73</v>
+        <v>21987.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -27083,7 +27086,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -27171,7 +27174,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>22070.73</v>
+        <v>22853.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27263,7 +27266,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>22070.73</v>
+        <v>22853.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27432,7 +27435,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -27535,7 +27538,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>23588.73</v>
+        <v>24371.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27627,7 +27630,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>23588.73</v>
+        <v>24371.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27811,7 +27814,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -27899,7 +27902,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>24454.73</v>
+        <v>25237.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28412,7 +28415,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>26400.73</v>
+        <v>27183.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28428,7 +28431,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26696.36</v>
+        <v>27479.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28444,7 +28447,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -29761,7 +29764,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="37">
         <v>68</v>
@@ -29943,7 +29946,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -30018,11 +30021,11 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="38" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -30042,7 +30045,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -30062,7 +30065,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -30138,7 +30141,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -30154,7 +30157,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -30248,7 +30251,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>24454.73</v>
+        <v>25237.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -30520,7 +30523,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>25099.73</v>
+        <v>25882.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30612,7 +30615,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>25099.73</v>
+        <v>25882.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30781,7 +30784,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -30796,7 +30799,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -30884,7 +30887,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>25805.73</v>
+        <v>26588.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -30976,7 +30979,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>25805.73</v>
+        <v>26588.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -31145,7 +31148,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -31248,7 +31251,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>26400.73</v>
+        <v>27183.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31768,7 +31771,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>28567.73</v>
+        <v>29350.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31784,7 +31787,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>28863.36</v>
+        <v>29646.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31800,7 +31803,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -33117,7 +33120,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="37">
         <v>68</v>
@@ -33299,7 +33302,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -33379,7 +33382,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -33399,7 +33402,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -33419,7 +33422,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -33495,7 +33498,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -33511,7 +33514,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -33605,7 +33608,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>26400.73</v>
+        <v>27183.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -33789,7 +33792,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -33877,7 +33880,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>27266.73</v>
+        <v>28049.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -33969,7 +33972,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>27266.73</v>
+        <v>28049.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -34138,7 +34141,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -34241,7 +34244,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>27701.73</v>
+        <v>28484.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -34333,7 +34336,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>27701.73</v>
+        <v>28484.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -34517,7 +34520,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -34605,7 +34608,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>28567.73</v>
+        <v>29350.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -35607,8 +35610,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -35703,7 +35706,7 @@
       </c>
       <c r="N3" s="196">
         <f>-C122</f>
-        <v>-333353.41</v>
+        <v>-7203.9</v>
       </c>
     </row>
     <row r="4" ht="35.25" customHeight="1" spans="1:14">
@@ -35735,7 +35738,7 @@
       </c>
       <c r="N4" s="196">
         <f ca="1">'April 2025 - June 2025'!C5</f>
-        <v>-331832.51</v>
+        <v>-5683</v>
       </c>
     </row>
     <row r="5" ht="35.25" customHeight="1" spans="1:14">
@@ -35767,7 +35770,7 @@
       </c>
       <c r="N5" s="196">
         <f ca="1">'July 2025 - September 2025'!C5</f>
-        <v>-329432.51</v>
+        <v>-3283</v>
       </c>
     </row>
     <row r="6" ht="35.25" customHeight="1" spans="1:14">
@@ -35799,7 +35802,7 @@
       </c>
       <c r="N6" s="196">
         <f ca="1">'October 2025 - December 2025'!C5</f>
-        <v>-327132.51</v>
+        <v>-983</v>
       </c>
     </row>
     <row r="7" ht="35.25" customHeight="1" spans="1:14">
@@ -35823,7 +35826,7 @@
       </c>
       <c r="J7" s="196">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>295.63</v>
+        <v>1227.73</v>
       </c>
       <c r="M7" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,12),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+12),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,15)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+14),"dd mmmm yyyy"))</f>
@@ -35831,7 +35834,7 @@
       </c>
       <c r="N7" s="196">
         <f ca="1">'January 2026 - March 2026'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="45" customHeight="1" spans="1:14">
@@ -35856,7 +35859,7 @@
       </c>
       <c r="J8" s="196">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>119.73</v>
+        <v>1202.73</v>
       </c>
       <c r="M8" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+15),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
@@ -35864,7 +35867,7 @@
       </c>
       <c r="N8" s="196">
         <f ca="1">'April 2026 - June 2026'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="39.75" customHeight="1" spans="1:14">
@@ -35888,7 +35891,7 @@
       </c>
       <c r="J9" s="196">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>185.73</v>
+        <v>1268.73</v>
       </c>
       <c r="M9" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+18),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,21)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+20),"dd mmmm yyyy"))</f>
@@ -35896,7 +35899,7 @@
       </c>
       <c r="N9" s="205">
         <f ca="1">'July 2026 - September 2026'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="35.25" customHeight="1" spans="1:14">
@@ -35920,7 +35923,7 @@
       </c>
       <c r="J10" s="196">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>110.73</v>
+        <v>1193.73</v>
       </c>
       <c r="M10" s="206" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
@@ -35928,7 +35931,7 @@
       </c>
       <c r="N10" s="196">
         <f ca="1">'October 2026 - December 2026'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" ht="35.25" customHeight="1" spans="1:14">
@@ -35953,7 +35956,7 @@
       </c>
       <c r="J11" s="196">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>176.73</v>
+        <v>1259.73</v>
       </c>
       <c r="M11" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+24),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
@@ -35961,7 +35964,7 @@
       </c>
       <c r="N11" s="200">
         <f ca="1">'January 2027 - March 2027'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" spans="1:14">
@@ -35985,7 +35988,7 @@
       </c>
       <c r="J12" s="196">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>151.73</v>
+        <v>1234.73</v>
       </c>
       <c r="M12" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+27),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
@@ -35993,7 +35996,7 @@
       </c>
       <c r="N12" s="200">
         <f ca="1">'April 2027 - June 2027'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" ht="35.25" customHeight="1" spans="1:14">
@@ -36017,7 +36020,7 @@
       </c>
       <c r="J13" s="196">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>167.73</v>
+        <v>1250.73</v>
       </c>
       <c r="M13" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -36025,7 +36028,7 @@
       </c>
       <c r="N13" s="200">
         <f ca="1">'July 2027 - September 2027'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" ht="35.25" customHeight="1" spans="1:14">
@@ -36049,7 +36052,7 @@
       </c>
       <c r="J14" s="200">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>112.73</v>
+        <v>1195.73</v>
       </c>
       <c r="M14" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -36057,7 +36060,7 @@
       </c>
       <c r="N14" s="200">
         <f ca="1">'October 2027 - December 2027'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" ht="35.25" customHeight="1" spans="1:14">
@@ -36081,7 +36084,7 @@
       </c>
       <c r="J15" s="200">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>295.73</v>
+        <v>1078.73</v>
       </c>
       <c r="M15" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -36089,7 +36092,7 @@
       </c>
       <c r="N15" s="200">
         <f ca="1">'January 2028 - March 2028'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="35.25" customHeight="1" spans="1:14">
@@ -36115,7 +36118,7 @@
       </c>
       <c r="J16" s="200">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>730.73</v>
+        <v>1513.73</v>
       </c>
       <c r="M16" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -36123,7 +36126,7 @@
       </c>
       <c r="N16" s="200">
         <f ca="1">'April 2028 - June 2028'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" ht="35.25" customHeight="1" spans="9:14">
@@ -36133,7 +36136,7 @@
       </c>
       <c r="J17" s="200">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>1596.73</v>
+        <v>2379.73</v>
       </c>
       <c r="M17" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -36141,7 +36144,7 @@
       </c>
       <c r="N17" s="200">
         <f ca="1">'July 2028 - September 2028'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" ht="35.25" customHeight="1" spans="9:14">
@@ -36151,7 +36154,7 @@
       </c>
       <c r="J18" s="200">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>2191.73</v>
+        <v>2974.73</v>
       </c>
       <c r="M18" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -36159,7 +36162,7 @@
       </c>
       <c r="N18" s="196">
         <f ca="1">'October 2028 - December 2028'!C5</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" ht="33" customHeight="1" spans="9:10">
@@ -36169,7 +36172,7 @@
       </c>
       <c r="J19" s="200">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>3980.73</v>
+        <v>4763.73</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -36179,7 +36182,7 @@
       </c>
       <c r="J20" s="200">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>4625.73</v>
+        <v>5408.73</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -36189,7 +36192,7 @@
       </c>
       <c r="J21" s="200">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>5491.73</v>
+        <v>6274.73</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -36209,7 +36212,7 @@
       </c>
       <c r="J22" s="200">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>5926.73</v>
+        <v>6709.73</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -36234,7 +36237,7 @@
       </c>
       <c r="J23" s="200">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>6792.73</v>
+        <v>7575.73</v>
       </c>
     </row>
     <row r="24" ht="33" customHeight="1" spans="1:10">
@@ -36253,7 +36256,7 @@
       </c>
       <c r="J24" s="200">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>7387.73</v>
+        <v>8170.73</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -36272,7 +36275,7 @@
       </c>
       <c r="J25" s="200">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>8093.73</v>
+        <v>8876.73</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -36291,7 +36294,7 @@
       </c>
       <c r="J26" s="200">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>8688.73</v>
+        <v>9471.73</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -36310,7 +36313,7 @@
       </c>
       <c r="J27" s="200">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>9554.73</v>
+        <v>10337.73</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -36329,7 +36332,7 @@
       </c>
       <c r="J28" s="200">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>9989.73</v>
+        <v>10772.73</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -36348,7 +36351,7 @@
       </c>
       <c r="J29" s="196">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>10855.73</v>
+        <v>11638.73</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -36370,7 +36373,7 @@
       </c>
       <c r="J30" s="202">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>12071.73</v>
+        <v>12854.73</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -36380,7 +36383,7 @@
       </c>
       <c r="J31" s="200">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>13939.73</v>
+        <v>14722.73</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -36390,7 +36393,7 @@
       </c>
       <c r="J32" s="200">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>15155.73</v>
+        <v>15938.73</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -36400,7 +36403,7 @@
       </c>
       <c r="J33" s="200">
         <f ca="1">'July 2027 - September 2027'!E136</f>
-        <v>15750.73</v>
+        <v>16533.73</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -36420,7 +36423,7 @@
       </c>
       <c r="J34" s="200">
         <f ca="1">'July 2027 - September 2027'!E163</f>
-        <v>16456.73</v>
+        <v>17239.73</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -36445,7 +36448,7 @@
       </c>
       <c r="J35" s="200">
         <f ca="1">'July 2027 - September 2027'!E190</f>
-        <v>17051.73</v>
+        <v>17834.73</v>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:10">
@@ -36468,7 +36471,7 @@
       </c>
       <c r="J36" s="200">
         <f ca="1">'October 2027 - December 2027'!E136</f>
-        <v>17917.73</v>
+        <v>18700.73</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -36487,7 +36490,7 @@
       </c>
       <c r="J37" s="200">
         <f ca="1">'October 2027 - December 2027'!E163</f>
-        <v>18352.73</v>
+        <v>19135.73</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -36506,7 +36509,7 @@
       </c>
       <c r="J38" s="200">
         <f ca="1">'October 2027 - December 2027'!E190</f>
-        <v>19218.73</v>
+        <v>20001.73</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -36525,7 +36528,7 @@
       </c>
       <c r="J39" s="200">
         <f ca="1">'January 2028 - March 2028'!E136</f>
-        <v>19863.73</v>
+        <v>20646.73</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -36544,7 +36547,7 @@
       </c>
       <c r="J40" s="200">
         <f ca="1">'January 2028 - March 2028'!E163</f>
-        <v>20569.73</v>
+        <v>21352.73</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -36563,7 +36566,7 @@
       </c>
       <c r="J41" s="200">
         <f ca="1">'January 2028 - March 2028'!E190</f>
-        <v>21204.73</v>
+        <v>21987.73</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -36585,7 +36588,7 @@
       </c>
       <c r="J42" s="200">
         <f ca="1">'April 2028 - June 2028'!E136</f>
-        <v>22070.73</v>
+        <v>22853.73</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -36595,7 +36598,7 @@
       </c>
       <c r="J43" s="200">
         <f ca="1">'April 2028 - June 2028'!E163</f>
-        <v>23588.73</v>
+        <v>24371.73</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -36605,7 +36608,7 @@
       </c>
       <c r="J44" s="200">
         <f ca="1">'April 2028 - June 2028'!E190</f>
-        <v>24454.73</v>
+        <v>25237.73</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -36615,7 +36618,7 @@
       </c>
       <c r="J45" s="200">
         <f ca="1">'July 2028 - September 2028'!E136</f>
-        <v>25099.73</v>
+        <v>25882.73</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -36635,7 +36638,7 @@
       </c>
       <c r="J46" s="200">
         <f ca="1">'July 2028 - September 2028'!E163</f>
-        <v>25805.73</v>
+        <v>26588.73</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -36660,7 +36663,7 @@
       </c>
       <c r="J47" s="200">
         <f ca="1">'July 2028 - September 2028'!E190</f>
-        <v>26400.73</v>
+        <v>27183.73</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -36683,7 +36686,7 @@
       </c>
       <c r="J48" s="200">
         <f ca="1">'October 2028 - December 2028'!E136</f>
-        <v>27266.73</v>
+        <v>28049.73</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -36702,7 +36705,7 @@
       </c>
       <c r="J49" s="200">
         <f ca="1">'October 2028 - December 2028'!E163</f>
-        <v>27701.73</v>
+        <v>28484.73</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -36721,7 +36724,7 @@
       </c>
       <c r="J50" s="196">
         <f ca="1">'October 2028 - December 2028'!E190</f>
-        <v>28567.73</v>
+        <v>29350.73</v>
       </c>
     </row>
     <row r="51" ht="41.1" customHeight="1" spans="1:7">
@@ -37271,7 +37274,7 @@
       </c>
       <c r="B116" s="184"/>
       <c r="C116" s="220">
-        <v>326149.51</v>
+        <v>0</v>
       </c>
       <c r="D116" s="14"/>
       <c r="E116" s="14"/>
@@ -37350,7 +37353,7 @@
       </c>
       <c r="C122" s="207">
         <f>SUM(C112:C121)</f>
-        <v>333353.41</v>
+        <v>7203.9</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -37360,7 +37363,7 @@
       </c>
       <c r="C123" s="37">
         <f>C122+C110</f>
-        <v>333753.41</v>
+        <v>7603.9</v>
       </c>
     </row>
     <row r="124" spans="5:5">
@@ -38585,8 +38588,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:E26"/>
+    <sheetView topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -38637,7 +38640,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>119.73</v>
+        <v>1202.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -38651,7 +38654,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>415.36</v>
+        <v>1498.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -38667,7 +38670,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-331832.51</v>
+        <v>-5683</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -38931,7 +38934,7 @@
       </c>
       <c r="E23" s="100"/>
       <c r="F23" s="7">
-        <v>0</v>
+        <v>1083</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="14"/>
@@ -39011,7 +39014,7 @@
       <c r="E28" s="45"/>
       <c r="F28" s="46">
         <f>SUM(F22:G27)</f>
-        <v>2553</v>
+        <v>3636</v>
       </c>
       <c r="G28" s="47"/>
       <c r="H28" s="14"/>
@@ -40019,7 +40022,7 @@
       </c>
       <c r="B88" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -40281,7 +40284,7 @@
       </c>
       <c r="C102" s="106" cm="1">
         <f ca="1" t="array" ref="C102">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E135")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E162")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E189")))+SUM(E122+E149+E176))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C116")</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="148"/>
@@ -40301,7 +40304,7 @@
       </c>
       <c r="C103" s="106" cm="1">
         <f ca="1" t="array" ref="C103">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E136")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E163")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E190")))+SUM(E123+E150+E177))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C117")</f>
-        <v>-932.1</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -40321,7 +40324,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E137")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E164")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E191")))+SUM(E124+E151+E178))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C118")</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -40397,7 +40400,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-331832.51</v>
+        <v>-5683</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -40413,7 +40416,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-332252.5</v>
+        <v>-6102.99</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -40978,10 +40981,12 @@
     <row r="151" ht="27" customHeight="1" spans="1:9">
       <c r="A151" s="63"/>
       <c r="B151" s="64"/>
-      <c r="C151" s="114"/>
+      <c r="C151" s="114" t="s">
+        <v>113</v>
+      </c>
       <c r="D151" s="149"/>
       <c r="E151" s="37">
-        <v>0</v>
+        <v>150.9</v>
       </c>
       <c r="F151" s="14"/>
       <c r="G151" s="14"/>
@@ -41044,7 +41049,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -41059,7 +41064,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -41074,7 +41079,7 @@
       <c r="A158" s="63"/>
       <c r="B158" s="64"/>
       <c r="C158" s="73" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D158" s="74"/>
       <c r="E158" s="87">
@@ -41089,7 +41094,7 @@
       <c r="A159" s="63"/>
       <c r="B159" s="64"/>
       <c r="C159" s="73" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D159" s="74"/>
       <c r="E159" s="87">
@@ -41104,7 +41109,7 @@
       <c r="A160" s="63"/>
       <c r="B160" s="64"/>
       <c r="C160" s="73" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D160" s="125"/>
       <c r="E160" s="87">
@@ -41153,7 +41158,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>295.63</v>
+        <v>1227.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -41237,14 +41242,14 @@
     </row>
     <row r="170" ht="24.75" customHeight="1" spans="1:9">
       <c r="A170" s="56" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>295.63</v>
+        <v>1227.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -41270,7 +41275,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -41333,15 +41338,13 @@
       <c r="H176" s="14"/>
       <c r="I176" s="48"/>
     </row>
-    <row r="177" ht="56" customHeight="1" spans="1:9">
+    <row r="177" ht="33" customHeight="1" spans="1:9">
       <c r="A177" s="63"/>
       <c r="B177" s="64"/>
-      <c r="C177" s="114" t="s">
-        <v>120</v>
-      </c>
+      <c r="C177" s="114"/>
       <c r="D177" s="149"/>
       <c r="E177" s="37">
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
@@ -41520,7 +41523,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>119.73</v>
+        <v>1202.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -42001,7 +42004,7 @@
   <sheetPr/>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" workbookViewId="0">
+    <sheetView topLeftCell="A112" workbookViewId="0">
       <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
@@ -42050,7 +42053,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>176.73</v>
+        <v>1259.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -42064,7 +42067,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>472.36</v>
+        <v>1555.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -42080,7 +42083,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-329432.51</v>
+        <v>-3283</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -43397,7 +43400,7 @@
       </c>
       <c r="B88" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -43659,7 +43662,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -43679,7 +43682,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>-932.1</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -43699,7 +43702,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -43775,7 +43778,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-329432.51</v>
+        <v>-3283</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -43791,7 +43794,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-329782.51</v>
+        <v>-3633</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -43885,7 +43888,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="89" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!E190")</f>
-        <v>119.73</v>
+        <v>1202.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -43911,7 +43914,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="37">
@@ -44071,7 +44074,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -44159,7 +44162,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>185.73</v>
+        <v>1268.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -44251,7 +44254,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>185.73</v>
+        <v>1268.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -44277,7 +44280,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="74" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D145" s="74"/>
       <c r="E145" s="37">
@@ -44525,7 +44528,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>110.73</v>
+        <v>1193.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -44617,7 +44620,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>110.73</v>
+        <v>1193.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -44643,7 +44646,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -44803,7 +44806,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -44891,7 +44894,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>176.73</v>
+        <v>1259.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -45421,8 +45424,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177:D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -45472,7 +45475,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>112.73</v>
+        <v>1195.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -45488,7 +45491,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>408.36</v>
+        <v>1491.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -45504,7 +45507,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-327132.51</v>
+        <v>-983</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -46821,7 +46824,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -47083,7 +47086,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -47103,7 +47106,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>-532.1</v>
+        <v>-683</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -47123,7 +47126,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -47199,7 +47202,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-327132.51</v>
+        <v>-983</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -47215,7 +47218,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-327482.51</v>
+        <v>-1333</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -47309,7 +47312,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!E190")</f>
-        <v>176.73</v>
+        <v>1259.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -47335,7 +47338,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="37">
@@ -47583,7 +47586,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>151.73</v>
+        <v>1234.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -47675,7 +47678,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>151.73</v>
+        <v>1234.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -47701,7 +47704,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="74" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D145" s="74"/>
       <c r="E145" s="37">
@@ -47861,7 +47864,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -47949,7 +47952,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>167.73</v>
+        <v>1250.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -48041,7 +48044,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>167.73</v>
+        <v>1250.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -48317,7 +48320,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>112.73</v>
+        <v>1195.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -48856,8 +48859,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -48908,7 +48911,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1596.73</v>
+        <v>2379.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -48924,7 +48927,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1892.36</v>
+        <v>2675.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -48940,7 +48943,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -50257,7 +50260,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -50439,7 +50442,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -50519,7 +50522,7 @@
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -50539,7 +50542,7 @@
       </c>
       <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -50559,7 +50562,7 @@
       </c>
       <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -50635,7 +50638,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -50651,7 +50654,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -50745,7 +50748,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>112.73</v>
+        <v>1195.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -50770,10 +50773,12 @@
     <row r="118" ht="24.75" customHeight="1" spans="1:9">
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
-      <c r="C118" s="74"/>
+      <c r="C118" s="74" t="s">
+        <v>128</v>
+      </c>
       <c r="D118" s="74"/>
       <c r="E118" s="87">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="F118" s="14"/>
       <c r="G118" s="14"/>
@@ -50836,7 +50841,7 @@
       <c r="A123" s="63"/>
       <c r="B123" s="64"/>
       <c r="C123" s="65" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D123" s="66"/>
       <c r="E123" s="37">
@@ -50931,7 +50936,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -51019,7 +51024,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>295.73</v>
+        <v>1078.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -51111,7 +51116,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>295.73</v>
+        <v>1078.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -51280,7 +51285,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -51383,7 +51388,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>730.73</v>
+        <v>1513.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -51475,7 +51480,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>730.73</v>
+        <v>1513.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -51659,7 +51664,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -51747,7 +51752,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1596.73</v>
+        <v>2379.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -52246,8 +52251,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -52296,7 +52301,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4625.73</v>
+        <v>5408.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -52312,7 +52317,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4921.36</v>
+        <v>5704.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52328,7 +52333,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -53642,14 +53647,14 @@
       <c r="H87" s="14"/>
       <c r="I87" s="48"/>
     </row>
-    <row r="88" ht="24.75" customHeight="1" spans="1:9">
+    <row r="88" ht="71" customHeight="1" spans="1:9">
       <c r="A88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="A88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A102")))</f>
         <v>Entertainment</v>
       </c>
-      <c r="B88" s="36" t="str" cm="1">
+      <c r="B88" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -53699,7 +53704,7 @@
       <c r="H90" s="14"/>
       <c r="I90" s="48"/>
     </row>
-    <row r="91" ht="24.75" customHeight="1" spans="1:9">
+    <row r="91" ht="55" customHeight="1" spans="1:9">
       <c r="A91" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A91">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A105"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A105")))</f>
         <v>Oxford Dictionary</v>
@@ -53831,7 +53836,7 @@
       </c>
       <c r="C98" s="106" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -53880,7 +53885,7 @@
       <c r="H100" s="14"/>
       <c r="I100" s="48"/>
     </row>
-    <row r="101" ht="24.75" customHeight="1" spans="1:9">
+    <row r="101" ht="50" customHeight="1" spans="1:9">
       <c r="A101" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A101">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A115"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A115")))</f>
         <v>Hong Kong Government Hospital Authority</v>
@@ -53900,7 +53905,7 @@
       <c r="H101" s="14"/>
       <c r="I101" s="48"/>
     </row>
-    <row r="102" ht="24.75" customHeight="1" spans="1:9">
+    <row r="102" ht="43" customHeight="1" spans="1:9">
       <c r="A102" s="38" t="str" cm="1">
         <f ca="1" t="array" ref="A102">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A116"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!A116")))</f>
         <v>Bankruptcy Department / Bank</v>
@@ -53911,7 +53916,7 @@
       </c>
       <c r="C102" s="106" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -53931,7 +53936,7 @@
       </c>
       <c r="C103" s="106" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -53951,7 +53956,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -54027,7 +54032,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -54043,7 +54048,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -54137,7 +54142,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>1596.73</v>
+        <v>2379.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -54306,7 +54311,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -54409,7 +54414,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2191.73</v>
+        <v>2974.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -54501,7 +54506,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>2191.73</v>
+        <v>2974.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -54670,7 +54675,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -54685,7 +54690,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -54773,7 +54778,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3980.73</v>
+        <v>4763.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -54865,7 +54870,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>3980.73</v>
+        <v>4763.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -55137,7 +55142,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4625.73</v>
+        <v>5408.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -55683,7 +55688,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6792.73</v>
+        <v>7575.73</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -55699,7 +55704,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7088.36</v>
+        <v>7871.36</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55715,7 +55720,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -55798,7 +55803,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="101" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -57034,7 +57039,7 @@
       </c>
       <c r="B88" s="36" t="str" cm="1">
         <f ca="1" t="array" ref="B88">IF((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102"))=0,"",(INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!B102")))</f>
-        <v>Sportify Music Paid For 7th of Each Month. Switch to Apple Music on the 6th of July 2025.</v>
+        <v>Sportify Music Paid For 7th of Each Month.</v>
       </c>
       <c r="C88" s="87">
         <v>68</v>
@@ -57216,7 +57221,7 @@
       </c>
       <c r="C98" s="106" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -57296,7 +57301,7 @@
       </c>
       <c r="C102" s="106" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>-326149.51</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -57316,7 +57321,7 @@
       </c>
       <c r="C103" s="106" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>150.9</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -57336,7 +57341,7 @@
       </c>
       <c r="C104" s="106" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>-150.9</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -57412,7 +57417,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-326449.51</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -57428,7 +57433,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-326799.51</v>
+        <v>-350</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -57522,7 +57527,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>4625.73</v>
+        <v>5408.73</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -57706,7 +57711,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -57794,7 +57799,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5491.73</v>
+        <v>6274.73</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -57886,7 +57891,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>5491.73</v>
+        <v>6274.73</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -58055,7 +58060,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -58158,7 +58163,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5926.73</v>
+        <v>6709.73</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -58250,7 +58255,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>5926.73</v>
+        <v>6709.73</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -58434,7 +58439,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -58522,7 +58527,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6792.73</v>
+        <v>7575.73</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: Top Up Value For Octopus.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Demo.xlsx
+++ b/Income And Expenses Forecast Demo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21480"/>
+    <workbookView windowHeight="21480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="136">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>~ Amazon Book Store ~ $150.9</t>
+  </si>
+  <si>
+    <t>~ Top Up For Octopus $50 (Don't need to Include)</t>
   </si>
   <si>
     <t xml:space="preserve">~ Payback $570 to Mom </t>
@@ -3045,7 +3048,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -6864,7 +6867,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -6879,7 +6882,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -7228,7 +7231,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -7243,7 +7246,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -7592,7 +7595,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -7607,7 +7610,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -10233,7 +10236,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -10248,7 +10251,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -10597,7 +10600,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -10612,7 +10615,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -10961,7 +10964,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -10976,7 +10979,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -13602,7 +13605,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -13617,7 +13620,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -13966,7 +13969,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -13981,7 +13984,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -14330,7 +14333,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -14345,7 +14348,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -16965,7 +16968,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -16980,7 +16983,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -17329,7 +17332,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -17344,7 +17347,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -17693,7 +17696,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -17708,7 +17711,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -20335,7 +20338,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -20350,7 +20353,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -20699,7 +20702,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -20714,7 +20717,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -21063,7 +21066,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -21078,7 +21081,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -23698,7 +23701,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -23713,7 +23716,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -24062,7 +24065,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -24077,7 +24080,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -24426,7 +24429,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -24441,7 +24444,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -27071,7 +27074,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -27086,7 +27089,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -27435,7 +27438,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -27450,7 +27453,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -27799,7 +27802,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -27814,7 +27817,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -30021,7 +30024,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -30420,7 +30423,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -30435,7 +30438,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -30784,7 +30787,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -30799,7 +30802,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -31148,7 +31151,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -31163,7 +31166,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -33777,7 +33780,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -33792,7 +33795,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -34141,7 +34144,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -34156,7 +34159,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -34505,7 +34508,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -34520,7 +34523,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -38588,8 +38591,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:G23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -40723,7 +40726,9 @@
     <row r="132" ht="24.75" customHeight="1" spans="1:9">
       <c r="A132" s="63"/>
       <c r="B132" s="64"/>
-      <c r="C132" s="74"/>
+      <c r="C132" s="74" t="s">
+        <v>112</v>
+      </c>
       <c r="D132" s="74"/>
       <c r="E132" s="87">
         <v>0</v>
@@ -40902,7 +40907,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="65" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D145" s="66"/>
       <c r="E145" s="37">
@@ -40982,7 +40987,7 @@
       <c r="A151" s="63"/>
       <c r="B151" s="64"/>
       <c r="C151" s="114" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D151" s="149"/>
       <c r="E151" s="37">
@@ -41049,7 +41054,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -41064,7 +41069,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -41079,7 +41084,7 @@
       <c r="A158" s="63"/>
       <c r="B158" s="64"/>
       <c r="C158" s="73" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D158" s="74"/>
       <c r="E158" s="87">
@@ -41094,7 +41099,7 @@
       <c r="A159" s="63"/>
       <c r="B159" s="64"/>
       <c r="C159" s="73" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D159" s="74"/>
       <c r="E159" s="87">
@@ -41109,7 +41114,7 @@
       <c r="A160" s="63"/>
       <c r="B160" s="64"/>
       <c r="C160" s="73" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D160" s="125"/>
       <c r="E160" s="87">
@@ -41242,7 +41247,7 @@
     </row>
     <row r="170" ht="24.75" customHeight="1" spans="1:9">
       <c r="A170" s="56" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
@@ -41275,7 +41280,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -41435,7 +41440,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -43914,7 +43919,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="37">
@@ -44059,7 +44064,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -44074,7 +44079,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -44280,7 +44285,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D145" s="74"/>
       <c r="E145" s="37">
@@ -44425,7 +44430,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -44440,7 +44445,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -44646,7 +44651,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -44791,7 +44796,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -44806,7 +44811,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -47338,7 +47343,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="37">
@@ -47498,7 +47503,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -47704,7 +47709,7 @@
       <c r="A145" s="63"/>
       <c r="B145" s="64"/>
       <c r="C145" s="74" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D145" s="74"/>
       <c r="E145" s="37">
@@ -47849,7 +47854,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -47864,7 +47869,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -48070,7 +48075,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -48137,7 +48142,7 @@
       <c r="A177" s="63"/>
       <c r="B177" s="64"/>
       <c r="C177" s="65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D177" s="66"/>
       <c r="E177" s="37">
@@ -48217,7 +48222,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -48232,7 +48237,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -50774,7 +50779,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="87">
@@ -50841,7 +50846,7 @@
       <c r="A123" s="63"/>
       <c r="B123" s="64"/>
       <c r="C123" s="65" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D123" s="66"/>
       <c r="E123" s="37">
@@ -50921,7 +50926,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -50936,7 +50941,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -51285,7 +51290,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -51300,7 +51305,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -51649,7 +51654,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -51664,7 +51669,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -54311,7 +54316,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -54326,7 +54331,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -54675,7 +54680,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -54690,7 +54695,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -55039,7 +55044,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -55054,7 +55059,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -55803,7 +55808,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="101" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -57696,7 +57701,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -57711,7 +57716,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -58060,7 +58065,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -58075,7 +58080,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -58424,7 +58429,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -58439,7 +58444,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">

</xml_diff>

<commit_message>
docs: Update Transport Expenses
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Demo.xlsx
+++ b/Income And Expenses Forecast Demo.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="138">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -467,7 +467,8 @@
 ~ Brought Bandage 4 inches X 2 ~ $20</t>
   </si>
   <si>
-    <t>~ Buy Cigarette Buds ~ $800</t>
+    <t>~ Buy Cigarette Buds ~ $800
+~ Transport for Cigarette Buds ~ $50</t>
   </si>
   <si>
     <t>~ Apple Music one month
@@ -503,6 +504,9 @@
   <si>
     <t>~ Food And Transport ~ $400
 ~ See the Doctor (Injection) ~ $19</t>
+  </si>
+  <si>
+    <t>~ Buy Cigarette Buds ~ $800</t>
   </si>
   <si>
     <t>- See the Doctor ~ $110
@@ -4855,7 +4859,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -4871,7 +4875,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>9436.22</v>
+        <v>9386.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4887,7 +4891,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>10628.44</v>
+        <v>10528.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -6708,7 +6712,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>7540.22</v>
+        <v>7490.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -6877,7 +6881,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -6980,7 +6984,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>8135.22</v>
+        <v>8085.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7072,7 +7076,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>8135.22</v>
+        <v>8085.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -7241,7 +7245,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -7256,7 +7260,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -7344,7 +7348,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>8841.22</v>
+        <v>8791.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -7436,7 +7440,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>8841.22</v>
+        <v>8791.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -7605,7 +7609,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -7708,7 +7712,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>9436.22</v>
+        <v>9386.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -8224,7 +8228,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -8240,7 +8244,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>11603.22</v>
+        <v>11553.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8256,7 +8260,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12795.44</v>
+        <v>12695.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10077,7 +10081,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>9436.22</v>
+        <v>9386.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -10261,7 +10265,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -10349,7 +10353,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>10302.22</v>
+        <v>10252.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -10441,7 +10445,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>10302.22</v>
+        <v>10252.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -10610,7 +10614,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -10713,7 +10717,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>10737.22</v>
+        <v>10687.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -10805,7 +10809,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>10737.22</v>
+        <v>10687.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -10989,7 +10993,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -11077,7 +11081,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11603.22</v>
+        <v>11553.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -11589,7 +11593,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -11605,7 +11609,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15903.22</v>
+        <v>15853.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -11621,7 +11625,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>17095.44</v>
+        <v>16995.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -13446,7 +13450,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>11603.22</v>
+        <v>11553.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -13630,7 +13634,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -13718,7 +13722,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12819.22</v>
+        <v>12769.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -13810,7 +13814,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>12819.22</v>
+        <v>12769.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -13979,7 +13983,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -14082,7 +14086,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14687.22</v>
+        <v>14637.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14174,7 +14178,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>14687.22</v>
+        <v>14637.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -14358,7 +14362,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -14446,7 +14450,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15903.22</v>
+        <v>15853.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -14956,7 +14960,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -14972,7 +14976,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17799.22</v>
+        <v>17749.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -14988,7 +14992,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18991.44</v>
+        <v>18891.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16809,7 +16813,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>15903.22</v>
+        <v>15853.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -16978,7 +16982,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -17081,7 +17085,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>16498.22</v>
+        <v>16448.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17173,7 +17177,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>16498.22</v>
+        <v>16448.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17342,7 +17346,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -17357,7 +17361,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -17445,7 +17449,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17204.22</v>
+        <v>17154.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -17537,7 +17541,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>17204.22</v>
+        <v>17154.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -17706,7 +17710,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -17809,7 +17813,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17799.22</v>
+        <v>17749.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18326,7 +18330,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18342,7 +18346,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19966.22</v>
+        <v>19916.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18358,7 +18362,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21158.44</v>
+        <v>21058.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -20179,7 +20183,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>17799.22</v>
+        <v>17749.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20363,7 +20367,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -20451,7 +20455,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>18665.22</v>
+        <v>18615.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20543,7 +20547,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>18665.22</v>
+        <v>18615.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -20712,7 +20716,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -20815,7 +20819,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19100.22</v>
+        <v>19050.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -20907,7 +20911,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>19100.22</v>
+        <v>19050.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21091,7 +21095,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -21179,7 +21183,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19966.22</v>
+        <v>19916.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -21689,7 +21693,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -21705,7 +21709,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>21952.22</v>
+        <v>21902.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -21721,7 +21725,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>23144.44</v>
+        <v>23044.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -23542,7 +23546,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>19966.22</v>
+        <v>19916.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23711,7 +23715,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -23814,7 +23818,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>20611.22</v>
+        <v>20561.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -23906,7 +23910,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>20611.22</v>
+        <v>20561.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24075,7 +24079,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -24090,7 +24094,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -24178,7 +24182,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>21317.22</v>
+        <v>21267.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24270,7 +24274,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>21317.22</v>
+        <v>21267.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24439,7 +24443,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -24542,7 +24546,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>21952.22</v>
+        <v>21902.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25058,7 +25062,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25074,7 +25078,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>25202.22</v>
+        <v>25152.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25090,7 +25094,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26394.44</v>
+        <v>26294.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -26915,7 +26919,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>21952.22</v>
+        <v>21902.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -27099,7 +27103,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -27187,7 +27191,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>22818.22</v>
+        <v>22768.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27279,7 +27283,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>22818.22</v>
+        <v>22768.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27448,7 +27452,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -27551,7 +27555,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>24336.22</v>
+        <v>24286.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27643,7 +27647,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>24336.22</v>
+        <v>24286.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27827,7 +27831,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -27915,7 +27919,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>25202.22</v>
+        <v>25152.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28412,7 +28416,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28428,7 +28432,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>27148.22</v>
+        <v>27098.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28444,7 +28448,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>28340.44</v>
+        <v>28240.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -30034,7 +30038,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="38" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -30264,7 +30268,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>25202.22</v>
+        <v>25152.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -30433,7 +30437,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -30536,7 +30540,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>25847.22</v>
+        <v>25797.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30628,7 +30632,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>25847.22</v>
+        <v>25797.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30797,7 +30801,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -30812,7 +30816,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -30900,7 +30904,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>26553.22</v>
+        <v>26503.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -30992,7 +30996,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>26553.22</v>
+        <v>26503.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -31161,7 +31165,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -31264,7 +31268,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>27148.22</v>
+        <v>27098.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31768,7 +31772,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31784,7 +31788,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>29315.22</v>
+        <v>29265.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31800,7 +31804,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>30507.44</v>
+        <v>30407.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -33621,7 +33625,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>27148.22</v>
+        <v>27098.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -33805,7 +33809,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -33893,7 +33897,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>28014.22</v>
+        <v>27964.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -33985,7 +33989,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>28014.22</v>
+        <v>27964.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -34154,7 +34158,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -34257,7 +34261,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>28449.22</v>
+        <v>28399.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -34349,7 +34353,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>28449.22</v>
+        <v>28399.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -34533,7 +34537,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -34621,7 +34625,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>29315.22</v>
+        <v>29265.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -35624,7 +35628,7 @@
   <dimension ref="A1:N204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -35703,7 +35707,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="187">
-        <v>100</v>
+        <v>997.1</v>
       </c>
       <c r="I3" s="195" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -35728,14 +35732,14 @@
         <v>36</v>
       </c>
       <c r="C4" s="159">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D4" s="161"/>
       <c r="E4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="187">
-        <v>900</v>
+        <v>100</v>
       </c>
       <c r="I4" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
@@ -35839,7 +35843,7 @@
       </c>
       <c r="J7" s="196">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="M7" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,12),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+12),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,15)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+14),"dd mmmm yyyy"))</f>
@@ -35872,7 +35876,7 @@
       </c>
       <c r="J8" s="196">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>1167.22</v>
+        <v>1117.22</v>
       </c>
       <c r="M8" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+15),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
@@ -35904,7 +35908,7 @@
       </c>
       <c r="J9" s="196">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>1233.22</v>
+        <v>1183.22</v>
       </c>
       <c r="M9" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+18),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,21)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+20),"dd mmmm yyyy"))</f>
@@ -35936,7 +35940,7 @@
       </c>
       <c r="J10" s="196">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>1158.22</v>
+        <v>1108.22</v>
       </c>
       <c r="M10" s="206" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
@@ -35969,7 +35973,7 @@
       </c>
       <c r="J11" s="196">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>1224.22</v>
+        <v>1174.22</v>
       </c>
       <c r="M11" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+24),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
@@ -36001,7 +36005,7 @@
       </c>
       <c r="J12" s="196">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>1199.22</v>
+        <v>1149.22</v>
       </c>
       <c r="M12" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+27),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
@@ -36033,7 +36037,7 @@
       </c>
       <c r="J13" s="196">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>1215.22</v>
+        <v>1165.22</v>
       </c>
       <c r="M13" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -36065,7 +36069,7 @@
       </c>
       <c r="J14" s="200">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>1160.22</v>
+        <v>1110.22</v>
       </c>
       <c r="M14" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -36097,7 +36101,7 @@
       </c>
       <c r="J15" s="200">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>1043.22</v>
+        <v>993.22</v>
       </c>
       <c r="M15" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -36115,7 +36119,7 @@
       </c>
       <c r="C16" s="165">
         <f>SUM(C3:C15)</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D16" s="166"/>
       <c r="E16" s="164" t="s">
@@ -36123,7 +36127,7 @@
       </c>
       <c r="F16" s="190">
         <f>SUM(F3:F15)</f>
-        <v>1095.12</v>
+        <v>1192.22</v>
       </c>
       <c r="I16" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -36131,7 +36135,7 @@
       </c>
       <c r="J16" s="200">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>1478.22</v>
+        <v>1428.22</v>
       </c>
       <c r="M16" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -36149,7 +36153,7 @@
       </c>
       <c r="J17" s="200">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>2344.22</v>
+        <v>2294.22</v>
       </c>
       <c r="M17" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -36167,7 +36171,7 @@
       </c>
       <c r="J18" s="200">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>2939.22</v>
+        <v>2889.22</v>
       </c>
       <c r="M18" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -36185,7 +36189,7 @@
       </c>
       <c r="J19" s="200">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>4728.22</v>
+        <v>4678.22</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -36195,7 +36199,7 @@
       </c>
       <c r="J20" s="200">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>5373.22</v>
+        <v>5323.22</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -36205,7 +36209,7 @@
       </c>
       <c r="J21" s="200">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>6239.22</v>
+        <v>6189.22</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -36225,7 +36229,7 @@
       </c>
       <c r="J22" s="200">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>6674.22</v>
+        <v>6624.22</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -36250,7 +36254,7 @@
       </c>
       <c r="J23" s="200">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>7540.22</v>
+        <v>7490.22</v>
       </c>
     </row>
     <row r="24" ht="33" customHeight="1" spans="1:10">
@@ -36269,7 +36273,7 @@
       </c>
       <c r="J24" s="200">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>8135.22</v>
+        <v>8085.22</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -36288,7 +36292,7 @@
       </c>
       <c r="J25" s="200">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>8841.22</v>
+        <v>8791.22</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -36307,7 +36311,7 @@
       </c>
       <c r="J26" s="200">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>9436.22</v>
+        <v>9386.22</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -36326,7 +36330,7 @@
       </c>
       <c r="J27" s="200">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>10302.22</v>
+        <v>10252.22</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -36345,7 +36349,7 @@
       </c>
       <c r="J28" s="200">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>10737.22</v>
+        <v>10687.22</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -36364,7 +36368,7 @@
       </c>
       <c r="J29" s="196">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>11603.22</v>
+        <v>11553.22</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -36386,7 +36390,7 @@
       </c>
       <c r="J30" s="202">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>12819.22</v>
+        <v>12769.22</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -36396,7 +36400,7 @@
       </c>
       <c r="J31" s="200">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>14687.22</v>
+        <v>14637.22</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -36406,7 +36410,7 @@
       </c>
       <c r="J32" s="200">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>15903.22</v>
+        <v>15853.22</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -36416,7 +36420,7 @@
       </c>
       <c r="J33" s="200">
         <f ca="1">'July 2027 - September 2027'!E136</f>
-        <v>16498.22</v>
+        <v>16448.22</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -36436,7 +36440,7 @@
       </c>
       <c r="J34" s="200">
         <f ca="1">'July 2027 - September 2027'!E163</f>
-        <v>17204.22</v>
+        <v>17154.22</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -36461,7 +36465,7 @@
       </c>
       <c r="J35" s="200">
         <f ca="1">'July 2027 - September 2027'!E190</f>
-        <v>17799.22</v>
+        <v>17749.22</v>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:10">
@@ -36484,7 +36488,7 @@
       </c>
       <c r="J36" s="200">
         <f ca="1">'October 2027 - December 2027'!E136</f>
-        <v>18665.22</v>
+        <v>18615.22</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -36503,7 +36507,7 @@
       </c>
       <c r="J37" s="200">
         <f ca="1">'October 2027 - December 2027'!E163</f>
-        <v>19100.22</v>
+        <v>19050.22</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -36522,7 +36526,7 @@
       </c>
       <c r="J38" s="200">
         <f ca="1">'October 2027 - December 2027'!E190</f>
-        <v>19966.22</v>
+        <v>19916.22</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -36541,7 +36545,7 @@
       </c>
       <c r="J39" s="200">
         <f ca="1">'January 2028 - March 2028'!E136</f>
-        <v>20611.22</v>
+        <v>20561.22</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -36560,7 +36564,7 @@
       </c>
       <c r="J40" s="200">
         <f ca="1">'January 2028 - March 2028'!E163</f>
-        <v>21317.22</v>
+        <v>21267.22</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -36579,7 +36583,7 @@
       </c>
       <c r="J41" s="200">
         <f ca="1">'January 2028 - March 2028'!E190</f>
-        <v>21952.22</v>
+        <v>21902.22</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -36601,7 +36605,7 @@
       </c>
       <c r="J42" s="200">
         <f ca="1">'April 2028 - June 2028'!E136</f>
-        <v>22818.22</v>
+        <v>22768.22</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -36611,7 +36615,7 @@
       </c>
       <c r="J43" s="200">
         <f ca="1">'April 2028 - June 2028'!E163</f>
-        <v>24336.22</v>
+        <v>24286.22</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -36621,7 +36625,7 @@
       </c>
       <c r="J44" s="200">
         <f ca="1">'April 2028 - June 2028'!E190</f>
-        <v>25202.22</v>
+        <v>25152.22</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -36631,7 +36635,7 @@
       </c>
       <c r="J45" s="200">
         <f ca="1">'July 2028 - September 2028'!E136</f>
-        <v>25847.22</v>
+        <v>25797.22</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -36651,7 +36655,7 @@
       </c>
       <c r="J46" s="200">
         <f ca="1">'July 2028 - September 2028'!E163</f>
-        <v>26553.22</v>
+        <v>26503.22</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -36676,7 +36680,7 @@
       </c>
       <c r="J47" s="200">
         <f ca="1">'July 2028 - September 2028'!E190</f>
-        <v>27148.22</v>
+        <v>27098.22</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -36699,7 +36703,7 @@
       </c>
       <c r="J48" s="200">
         <f ca="1">'October 2028 - December 2028'!E136</f>
-        <v>28014.22</v>
+        <v>27964.22</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -36718,7 +36722,7 @@
       </c>
       <c r="J49" s="200">
         <f ca="1">'October 2028 - December 2028'!E163</f>
-        <v>28449.22</v>
+        <v>28399.22</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -36737,7 +36741,7 @@
       </c>
       <c r="J50" s="196">
         <f ca="1">'October 2028 - December 2028'!E190</f>
-        <v>29315.22</v>
+        <v>29265.22</v>
       </c>
     </row>
     <row r="51" ht="41.1" customHeight="1" spans="1:7">
@@ -38601,8 +38605,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -38639,7 +38643,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -38653,7 +38657,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1167.22</v>
+        <v>1117.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -38667,7 +38671,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2359.44</v>
+        <v>2259.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -41073,15 +41077,15 @@
       <c r="H156" s="14"/>
       <c r="I156" s="48"/>
     </row>
-    <row r="157" ht="24.75" customHeight="1" spans="1:9">
+    <row r="157" ht="43" customHeight="1" spans="1:9">
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
-      <c r="C157" s="74" t="s">
+      <c r="C157" s="73" t="s">
         <v>117</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -41171,7 +41175,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -41262,7 +41266,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -41429,7 +41433,7 @@
       <c r="H182" s="14"/>
       <c r="I182" s="48"/>
     </row>
-    <row r="183" ht="51" customHeight="1" spans="1:9">
+    <row r="183" ht="71" customHeight="1" spans="1:9">
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
@@ -41536,7 +41540,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1167.22</v>
+        <v>1117.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -42060,7 +42064,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -42074,7 +42078,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1224.22</v>
+        <v>1174.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -42088,7 +42092,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2416.44</v>
+        <v>2316.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43909,7 +43913,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="89" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!E190")</f>
-        <v>1167.22</v>
+        <v>1117.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -44095,7 +44099,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -44183,7 +44187,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1233.22</v>
+        <v>1183.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -44275,7 +44279,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>1233.22</v>
+        <v>1183.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -44446,7 +44450,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -44549,7 +44553,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1158.22</v>
+        <v>1108.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -44641,7 +44645,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>1158.22</v>
+        <v>1108.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -44827,7 +44831,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -44915,7 +44919,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1224.22</v>
+        <v>1174.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -45480,7 +45484,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -45496,7 +45500,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1160.22</v>
+        <v>1110.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -45512,7 +45516,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2352.44</v>
+        <v>2252.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -47333,7 +47337,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!E190")</f>
-        <v>1224.22</v>
+        <v>1174.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -47607,7 +47611,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1199.22</v>
+        <v>1149.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -47699,7 +47703,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>1199.22</v>
+        <v>1149.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -47870,7 +47874,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -47885,7 +47889,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -47973,7 +47977,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1215.22</v>
+        <v>1165.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -48065,7 +48069,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>1215.22</v>
+        <v>1165.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -48091,7 +48095,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -48158,7 +48162,7 @@
       <c r="A177" s="63"/>
       <c r="B177" s="64"/>
       <c r="C177" s="65" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D177" s="66"/>
       <c r="E177" s="37">
@@ -48238,7 +48242,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -48341,7 +48345,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1160.22</v>
+        <v>1110.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -48916,7 +48920,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48932,7 +48936,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>2344.22</v>
+        <v>2294.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -48948,7 +48952,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3536.44</v>
+        <v>3436.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -50769,7 +50773,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>1160.22</v>
+        <v>1110.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -50795,7 +50799,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="87">
@@ -50862,7 +50866,7 @@
       <c r="A123" s="63"/>
       <c r="B123" s="64"/>
       <c r="C123" s="65" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D123" s="66"/>
       <c r="E123" s="37">
@@ -50957,7 +50961,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -51045,7 +51049,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1043.22</v>
+        <v>993.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -51137,7 +51141,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>1043.22</v>
+        <v>993.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -51306,7 +51310,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -51409,7 +51413,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1478.22</v>
+        <v>1428.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -51501,7 +51505,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>1478.22</v>
+        <v>1428.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -51685,7 +51689,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -51773,7 +51777,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>2344.22</v>
+        <v>2294.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -52306,7 +52310,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -52322,7 +52326,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>5373.22</v>
+        <v>5323.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -52338,7 +52342,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6565.44</v>
+        <v>6465.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -54163,7 +54167,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>2344.22</v>
+        <v>2294.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -54332,7 +54336,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -54435,7 +54439,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2939.22</v>
+        <v>2889.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -54527,7 +54531,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>2939.22</v>
+        <v>2889.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -54696,7 +54700,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -54711,7 +54715,7 @@
       <c r="A157" s="63"/>
       <c r="B157" s="64"/>
       <c r="C157" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D157" s="74"/>
       <c r="E157" s="87">
@@ -54799,7 +54803,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4728.22</v>
+        <v>4678.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -54891,7 +54895,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>4728.22</v>
+        <v>4678.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -55060,7 +55064,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -55163,7 +55167,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5373.22</v>
+        <v>5323.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -55693,7 +55697,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1192.22</v>
+        <v>1142.22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -55709,7 +55713,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>7540.22</v>
+        <v>7490.22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -55725,7 +55729,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>8732.44</v>
+        <v>8632.44</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55824,7 +55828,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="101" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -57548,7 +57552,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>5373.22</v>
+        <v>5323.22</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -57732,7 +57736,7 @@
       <c r="A130" s="63"/>
       <c r="B130" s="64"/>
       <c r="C130" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D130" s="74"/>
       <c r="E130" s="87">
@@ -57820,7 +57824,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>6239.22</v>
+        <v>6189.22</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -57912,7 +57916,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>6239.22</v>
+        <v>6189.22</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -58081,7 +58085,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -58184,7 +58188,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>6674.22</v>
+        <v>6624.22</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -58276,7 +58280,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>6674.22</v>
+        <v>6624.22</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -58460,7 +58464,7 @@
       <c r="A184" s="63"/>
       <c r="B184" s="64"/>
       <c r="C184" s="74" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D184" s="74"/>
       <c r="E184" s="87">
@@ -58548,7 +58552,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>7540.22</v>
+        <v>7490.22</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: Payback Mom Installment updated.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Demo.xlsx
+++ b/Income And Expenses Forecast Demo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21480" activeTab="2"/>
+    <workbookView windowHeight="21480"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="148">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -477,7 +477,7 @@
 ~ Transport for Cigarette Buds ~ $50</t>
   </si>
   <si>
-    <t>~ Apple Music one month
+    <t>~ Apple Music 2 month
 ~ Top Up For Mobile And Comunication ~ $0.6
 ~ 20th May 2025 - Top Up For Octopus $50 (Don't need to Include)
 ~ 23rd May 2025 - Top Up For Octopus $100 (Don't need to Include)</t>
@@ -514,13 +514,14 @@
 ~ Pharmacy Sentalize Solutions ~ $20
 ~ Round Trip to East Kowloon Hospital ~ $4
 ~ Watsons ~ Asprin Like medicine ~ $49
-~ Wellcome ~ Plastic bag ~ $1</t>
+~ Wellcome ~ Plastic bag ~ $1
+~ Spring Sunday Aspirin tablets ~ $276.04</t>
   </si>
   <si>
     <t>Balance Brought Forward From July 2024</t>
   </si>
   <si>
-    <t>~ Payback $1100 to Mom</t>
+    <t>~ Payback $700 to Mom</t>
   </si>
   <si>
     <t>- See the Doctor ~ $110
@@ -540,7 +541,7 @@
     <t>~ Buy Cigarette Buds ~ $650</t>
   </si>
   <si>
-    <t>~ Payback $1000 to Mom</t>
+    <t>~ Payback $800 to Mom</t>
   </si>
   <si>
     <t>- See the Doctor ~ $110
@@ -548,7 +549,7 @@
 ~ See the Doctor For Blood Pressure ~ $50</t>
   </si>
   <si>
-    <t>~ Payback $800 to Mom</t>
+    <t>~ Payback $1000 to Mom</t>
   </si>
   <si>
     <t>~ Payback $770 to Mom</t>
@@ -562,7 +563,7 @@
 ~ See the Doctor For Blood Pressure ~ $50</t>
   </si>
   <si>
-    <t>~ Payback $250 to Mom</t>
+    <t>~ Payback $350 to Mom</t>
   </si>
   <si>
     <t>~ Payback $400 for Mom Air Ticket</t>
@@ -570,6 +571,9 @@
   <si>
     <t>- See the Doctor ~ $240
 - Buy Cigarette Buds ~ $650</t>
+  </si>
+  <si>
+    <t>~ Payback $500 to Mom</t>
   </si>
   <si>
     <t>~ Payback $483 for Mom Air Ticket</t>
@@ -3110,7 +3114,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -4907,7 +4911,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -4923,7 +4927,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10897.02</v>
+        <v>10552.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4939,7 +4943,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11570.04</v>
+        <v>10881.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -6760,7 +6764,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>8701.02</v>
+        <v>8356.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -6929,7 +6933,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -7032,7 +7036,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>9446.02</v>
+        <v>9101.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7124,7 +7128,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>9446.02</v>
+        <v>9101.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -7293,7 +7297,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -7396,7 +7400,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>10302.02</v>
+        <v>9957.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -7488,7 +7492,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>10302.02</v>
+        <v>9957.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -7657,7 +7661,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -7760,7 +7764,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10897.02</v>
+        <v>10552.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -8276,7 +8280,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -8292,7 +8296,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>13514.02</v>
+        <v>13169.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8308,7 +8312,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>14187.04</v>
+        <v>13498.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10129,7 +10133,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>10897.02</v>
+        <v>10552.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -10401,7 +10405,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>11913.02</v>
+        <v>11568.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -10493,7 +10497,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>11913.02</v>
+        <v>11568.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -10662,7 +10666,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -10765,7 +10769,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>12498.02</v>
+        <v>12153.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -10857,7 +10861,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>12498.02</v>
+        <v>12153.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11129,7 +11133,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>13514.02</v>
+        <v>13169.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -11641,7 +11645,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -11657,7 +11661,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>18264.02</v>
+        <v>17919.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -11673,7 +11677,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18937.04</v>
+        <v>18248.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -13498,7 +13502,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>13514.02</v>
+        <v>13169.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -13770,7 +13774,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>14880.02</v>
+        <v>14535.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -13862,7 +13866,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>14880.02</v>
+        <v>14535.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14031,7 +14035,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -14134,7 +14138,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>16898.02</v>
+        <v>16553.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14226,7 +14230,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>16898.02</v>
+        <v>16553.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -14498,7 +14502,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>18264.02</v>
+        <v>17919.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15008,7 +15012,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15024,7 +15028,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>20460.02</v>
+        <v>20115.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15040,7 +15044,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21133.04</v>
+        <v>20444.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16861,7 +16865,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>18264.02</v>
+        <v>17919.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17030,7 +17034,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -17133,7 +17137,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19009.02</v>
+        <v>18664.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17225,7 +17229,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>19009.02</v>
+        <v>18664.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17394,7 +17398,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -17497,7 +17501,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19865.02</v>
+        <v>19520.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -17589,7 +17593,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>19865.02</v>
+        <v>19520.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -17758,7 +17762,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -17861,7 +17865,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>20460.02</v>
+        <v>20115.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18378,7 +18382,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18394,7 +18398,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>23077.02</v>
+        <v>22732.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18410,7 +18414,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>23750.04</v>
+        <v>23061.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -20231,7 +20235,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>20460.02</v>
+        <v>20115.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20503,7 +20507,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>21476.02</v>
+        <v>21131.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20595,7 +20599,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>21476.02</v>
+        <v>21131.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -20764,7 +20768,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -20867,7 +20871,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>22061.02</v>
+        <v>21716.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -20959,7 +20963,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>22061.02</v>
+        <v>21716.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21231,7 +21235,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>23077.02</v>
+        <v>22732.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -21741,7 +21745,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -21757,7 +21761,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>25363.02</v>
+        <v>25018.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -21773,7 +21777,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26036.04</v>
+        <v>25347.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -23594,7 +23598,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>23077.02</v>
+        <v>22732.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23866,7 +23870,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>23872.02</v>
+        <v>23527.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -23958,7 +23962,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>23872.02</v>
+        <v>23527.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24127,7 +24131,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -24230,7 +24234,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>24728.02</v>
+        <v>24383.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24322,7 +24326,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>24728.02</v>
+        <v>24383.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24491,7 +24495,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -24594,7 +24598,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>25363.02</v>
+        <v>25018.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25110,7 +25114,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25126,7 +25130,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>29063.02</v>
+        <v>28718.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25142,7 +25146,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>29736.04</v>
+        <v>29047.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -26967,7 +26971,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>25363.02</v>
+        <v>25018.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -27239,7 +27243,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>26379.02</v>
+        <v>26034.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27331,7 +27335,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>26379.02</v>
+        <v>26034.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27500,7 +27504,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -27603,7 +27607,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>28047.02</v>
+        <v>27702.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27695,7 +27699,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>28047.02</v>
+        <v>27702.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27967,7 +27971,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>29063.02</v>
+        <v>28718.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28464,7 +28468,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28480,7 +28484,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>31459.02</v>
+        <v>31114.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28496,7 +28500,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>32132.04</v>
+        <v>31443.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -30086,7 +30090,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="38" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -30316,7 +30320,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>29063.02</v>
+        <v>28718.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -30588,7 +30592,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>29858.02</v>
+        <v>29513.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30680,7 +30684,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>29858.02</v>
+        <v>29513.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30849,7 +30853,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -30952,7 +30956,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>30714.02</v>
+        <v>30369.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -31044,7 +31048,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>30714.02</v>
+        <v>30369.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -31213,7 +31217,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -31316,7 +31320,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>31459.02</v>
+        <v>31114.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31820,7 +31824,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31836,7 +31840,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34076.02</v>
+        <v>33731.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31852,7 +31856,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>34749.04</v>
+        <v>34060.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -33673,7 +33677,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>31459.02</v>
+        <v>31114.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -33945,7 +33949,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>32475.02</v>
+        <v>32130.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34037,7 +34041,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>32475.02</v>
+        <v>32130.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -34206,7 +34210,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -34309,7 +34313,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>33060.02</v>
+        <v>32715.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -34401,7 +34405,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>33060.02</v>
+        <v>32715.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -34673,7 +34677,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34076.02</v>
+        <v>33731.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -35675,8 +35679,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -35787,7 +35791,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="187">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I4" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
@@ -35803,7 +35807,7 @@
       </c>
       <c r="N4" s="196">
         <f ca="1">'April 2025 - June 2025'!C5</f>
-        <v>-5953</v>
+        <v>-6353</v>
       </c>
     </row>
     <row r="5" ht="35.25" customHeight="1" spans="1:14">
@@ -35835,7 +35839,7 @@
       </c>
       <c r="N5" s="196">
         <f ca="1">'July 2025 - September 2025'!C5</f>
-        <v>-2903</v>
+        <v>-3503</v>
       </c>
     </row>
     <row r="6" ht="35.25" customHeight="1" spans="1:14">
@@ -35867,7 +35871,7 @@
       </c>
       <c r="N6" s="196">
         <f ca="1">'October 2025 - December 2025'!C5</f>
-        <v>-483</v>
+        <v>-983</v>
       </c>
     </row>
     <row r="7" ht="35.25" customHeight="1" spans="1:14">
@@ -35876,7 +35880,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="159">
-        <v>636.2</v>
+        <v>292.16</v>
       </c>
       <c r="D7" s="161"/>
       <c r="E7" s="5" t="s">
@@ -35891,7 +35895,7 @@
       </c>
       <c r="J7" s="196">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="M7" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,12),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+12),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,15)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+14),"dd mmmm yyyy"))</f>
@@ -35924,7 +35928,7 @@
       </c>
       <c r="J8" s="196">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>498.02</v>
+        <v>553.98</v>
       </c>
       <c r="M8" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+15),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
@@ -35956,7 +35960,7 @@
       </c>
       <c r="J9" s="196">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>464.02</v>
+        <v>519.98</v>
       </c>
       <c r="M9" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+18),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,21)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+20),"dd mmmm yyyy"))</f>
@@ -35988,7 +35992,7 @@
       </c>
       <c r="J10" s="196">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>339.02</v>
+        <v>594.98</v>
       </c>
       <c r="M10" s="206" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
@@ -36021,7 +36025,7 @@
       </c>
       <c r="J11" s="196">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>355.02</v>
+        <v>610.98</v>
       </c>
       <c r="M11" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+24),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
@@ -36053,7 +36057,7 @@
       </c>
       <c r="J12" s="196">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>480.02</v>
+        <v>735.98</v>
       </c>
       <c r="M12" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+27),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
@@ -36085,7 +36089,7 @@
       </c>
       <c r="J13" s="196">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>476.02</v>
+        <v>731.98</v>
       </c>
       <c r="M13" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -36117,7 +36121,7 @@
       </c>
       <c r="J14" s="200">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>621.02</v>
+        <v>776.98</v>
       </c>
       <c r="M14" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -36149,7 +36153,7 @@
       </c>
       <c r="J15" s="200">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>1154.02</v>
+        <v>809.98</v>
       </c>
       <c r="M15" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -36167,7 +36171,7 @@
       </c>
       <c r="C16" s="165">
         <f>SUM(C3:C15)</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D16" s="166"/>
       <c r="E16" s="164" t="s">
@@ -36175,7 +36179,7 @@
       </c>
       <c r="F16" s="190">
         <f>SUM(F3:F15)</f>
-        <v>723.02</v>
+        <v>673.02</v>
       </c>
       <c r="I16" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -36183,7 +36187,7 @@
       </c>
       <c r="J16" s="200">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>1739.02</v>
+        <v>1394.98</v>
       </c>
       <c r="M16" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -36201,7 +36205,7 @@
       </c>
       <c r="J17" s="200">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>2755.02</v>
+        <v>2410.98</v>
       </c>
       <c r="M17" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -36219,7 +36223,7 @@
       </c>
       <c r="J18" s="200">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>3500.02</v>
+        <v>3155.98</v>
       </c>
       <c r="M18" s="197" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -36237,7 +36241,7 @@
       </c>
       <c r="J19" s="200">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>5439.02</v>
+        <v>5094.98</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -36247,7 +36251,7 @@
       </c>
       <c r="J20" s="200">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>6084.02</v>
+        <v>5739.98</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -36257,7 +36261,7 @@
       </c>
       <c r="J21" s="200">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>7100.02</v>
+        <v>6755.98</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -36277,7 +36281,7 @@
       </c>
       <c r="J22" s="200">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>7685.02</v>
+        <v>7340.98</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -36302,7 +36306,7 @@
       </c>
       <c r="J23" s="200">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>8701.02</v>
+        <v>8356.98</v>
       </c>
     </row>
     <row r="24" ht="33" customHeight="1" spans="1:10">
@@ -36321,7 +36325,7 @@
       </c>
       <c r="J24" s="200">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>9446.02</v>
+        <v>9101.98</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -36340,7 +36344,7 @@
       </c>
       <c r="J25" s="200">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>10302.02</v>
+        <v>9957.98</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -36359,7 +36363,7 @@
       </c>
       <c r="J26" s="200">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>10897.02</v>
+        <v>10552.98</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -36378,7 +36382,7 @@
       </c>
       <c r="J27" s="200">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>11913.02</v>
+        <v>11568.98</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -36397,7 +36401,7 @@
       </c>
       <c r="J28" s="200">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>12498.02</v>
+        <v>12153.98</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -36416,7 +36420,7 @@
       </c>
       <c r="J29" s="196">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>13514.02</v>
+        <v>13169.98</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -36438,7 +36442,7 @@
       </c>
       <c r="J30" s="202">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>14880.02</v>
+        <v>14535.98</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -36448,7 +36452,7 @@
       </c>
       <c r="J31" s="200">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>16898.02</v>
+        <v>16553.98</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -36458,7 +36462,7 @@
       </c>
       <c r="J32" s="200">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>18264.02</v>
+        <v>17919.98</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -36468,7 +36472,7 @@
       </c>
       <c r="J33" s="200">
         <f ca="1">'July 2027 - September 2027'!E136</f>
-        <v>19009.02</v>
+        <v>18664.98</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -36488,7 +36492,7 @@
       </c>
       <c r="J34" s="200">
         <f ca="1">'July 2027 - September 2027'!E163</f>
-        <v>19865.02</v>
+        <v>19520.98</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -36513,7 +36517,7 @@
       </c>
       <c r="J35" s="200">
         <f ca="1">'July 2027 - September 2027'!E190</f>
-        <v>20460.02</v>
+        <v>20115.98</v>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:10">
@@ -36536,7 +36540,7 @@
       </c>
       <c r="J36" s="200">
         <f ca="1">'October 2027 - December 2027'!E136</f>
-        <v>21476.02</v>
+        <v>21131.98</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -36555,7 +36559,7 @@
       </c>
       <c r="J37" s="200">
         <f ca="1">'October 2027 - December 2027'!E163</f>
-        <v>22061.02</v>
+        <v>21716.98</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -36574,7 +36578,7 @@
       </c>
       <c r="J38" s="200">
         <f ca="1">'October 2027 - December 2027'!E190</f>
-        <v>23077.02</v>
+        <v>22732.98</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -36593,7 +36597,7 @@
       </c>
       <c r="J39" s="200">
         <f ca="1">'January 2028 - March 2028'!E136</f>
-        <v>23872.02</v>
+        <v>23527.98</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -36612,7 +36616,7 @@
       </c>
       <c r="J40" s="200">
         <f ca="1">'January 2028 - March 2028'!E163</f>
-        <v>24728.02</v>
+        <v>24383.98</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -36631,7 +36635,7 @@
       </c>
       <c r="J41" s="200">
         <f ca="1">'January 2028 - March 2028'!E190</f>
-        <v>25363.02</v>
+        <v>25018.98</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -36653,7 +36657,7 @@
       </c>
       <c r="J42" s="200">
         <f ca="1">'April 2028 - June 2028'!E136</f>
-        <v>26379.02</v>
+        <v>26034.98</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -36663,7 +36667,7 @@
       </c>
       <c r="J43" s="200">
         <f ca="1">'April 2028 - June 2028'!E163</f>
-        <v>28047.02</v>
+        <v>27702.98</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -36673,7 +36677,7 @@
       </c>
       <c r="J44" s="200">
         <f ca="1">'April 2028 - June 2028'!E190</f>
-        <v>29063.02</v>
+        <v>28718.98</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -36683,7 +36687,7 @@
       </c>
       <c r="J45" s="200">
         <f ca="1">'July 2028 - September 2028'!E136</f>
-        <v>29858.02</v>
+        <v>29513.98</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -36703,7 +36707,7 @@
       </c>
       <c r="J46" s="200">
         <f ca="1">'July 2028 - September 2028'!E163</f>
-        <v>30714.02</v>
+        <v>30369.98</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -36728,7 +36732,7 @@
       </c>
       <c r="J47" s="200">
         <f ca="1">'July 2028 - September 2028'!E190</f>
-        <v>31459.02</v>
+        <v>31114.98</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -36751,7 +36755,7 @@
       </c>
       <c r="J48" s="200">
         <f ca="1">'October 2028 - December 2028'!E136</f>
-        <v>32475.02</v>
+        <v>32130.98</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -36770,7 +36774,7 @@
       </c>
       <c r="J49" s="200">
         <f ca="1">'October 2028 - December 2028'!E163</f>
-        <v>33060.02</v>
+        <v>32715.98</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -36789,7 +36793,7 @@
       </c>
       <c r="J50" s="196">
         <f ca="1">'October 2028 - December 2028'!E190</f>
-        <v>34076.02</v>
+        <v>33731.98</v>
       </c>
     </row>
     <row r="51" ht="41.1" customHeight="1" spans="1:7">
@@ -38653,8 +38657,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="F160" sqref="F160"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -38691,7 +38695,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -38705,7 +38709,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>498.02</v>
+        <v>553.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -38719,7 +38723,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1171.04</v>
+        <v>882.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -38735,7 +38739,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-5953</v>
+        <v>-6353</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -40274,7 +40278,7 @@
       </c>
       <c r="C98" s="106" cm="1">
         <f ca="1" t="array" ref="C98">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E131")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E158")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E185")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C112")</f>
-        <v>-4870</v>
+        <v>-5270</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -40469,7 +40473,7 @@
       </c>
       <c r="C108" s="106">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-5953</v>
+        <v>-6353</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -40485,7 +40489,7 @@
       </c>
       <c r="C109" s="106">
         <f ca="1">C108-C96</f>
-        <v>-6372.99</v>
+        <v>-6772.99</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -41152,7 +41156,7 @@
       </c>
       <c r="D158" s="74"/>
       <c r="E158" s="87">
-        <v>68.6</v>
+        <v>136.6</v>
       </c>
       <c r="F158" s="14"/>
       <c r="G158" s="14"/>
@@ -41182,7 +41186,7 @@
       </c>
       <c r="D160" s="125"/>
       <c r="E160" s="87">
-        <v>344</v>
+        <v>620.04</v>
       </c>
       <c r="F160" s="14"/>
       <c r="G160" s="14"/>
@@ -41227,7 +41231,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -41318,7 +41322,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -41348,7 +41352,7 @@
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="F172" s="14"/>
       <c r="G172" s="14"/>
@@ -41592,7 +41596,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>498.02</v>
+        <v>553.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -42082,7 +42086,7 @@
   <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+      <selection activeCell="G155" sqref="G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -42116,7 +42120,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -42130,7 +42134,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>355.02</v>
+        <v>610.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -42144,7 +42148,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1028.04</v>
+        <v>939.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -42160,7 +42164,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-2903</v>
+        <v>-3503</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -43659,7 +43663,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-1820</v>
+        <v>-2420</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -43855,7 +43859,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-2903</v>
+        <v>-3503</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -43871,7 +43875,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-3253</v>
+        <v>-3853</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -43965,7 +43969,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="89" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!E190")</f>
-        <v>498.02</v>
+        <v>553.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -44239,7 +44243,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>464.02</v>
+        <v>519.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -44331,7 +44335,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>464.02</v>
+        <v>519.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -44361,7 +44365,7 @@
       </c>
       <c r="D145" s="74"/>
       <c r="E145" s="37">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F145" s="14"/>
       <c r="G145" s="14"/>
@@ -44605,7 +44609,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>339.02</v>
+        <v>594.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -44697,7 +44701,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>339.02</v>
+        <v>594.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -44723,7 +44727,7 @@
       <c r="A172" s="63"/>
       <c r="B172" s="64"/>
       <c r="C172" s="74" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
@@ -44971,7 +44975,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>355.02</v>
+        <v>610.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -45501,8 +45505,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="G180" sqref="G180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -45536,7 +45540,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -45552,7 +45556,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>621.02</v>
+        <v>776.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -45568,7 +45572,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1294.04</v>
+        <v>1105.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -45584,7 +45588,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-483</v>
+        <v>-983</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -47083,7 +47087,7 @@
       </c>
       <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="96"/>
@@ -47279,7 +47283,7 @@
       </c>
       <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-483</v>
+        <v>-983</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -47295,7 +47299,7 @@
       </c>
       <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>-833</v>
+        <v>-1333</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -47389,7 +47393,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!E190")</f>
-        <v>355.02</v>
+        <v>610.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -47415,7 +47419,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="74" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D118" s="74"/>
       <c r="E118" s="37">
@@ -47663,7 +47667,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>480.02</v>
+        <v>735.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -47755,7 +47759,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>480.02</v>
+        <v>735.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -48031,7 +48035,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>476.02</v>
+        <v>731.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -48123,7 +48127,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>476.02</v>
+        <v>731.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -48153,7 +48157,7 @@
       </c>
       <c r="D172" s="74"/>
       <c r="E172" s="37">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="F172" s="14"/>
       <c r="G172" s="14"/>
@@ -48399,7 +48403,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>621.02</v>
+        <v>776.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -48938,8 +48942,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157:D157"/>
+    <sheetView topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -48974,7 +48978,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48990,7 +48994,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>2755.02</v>
+        <v>2410.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -49006,7 +49010,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3428.04</v>
+        <v>2739.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -50827,7 +50831,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>621.02</v>
+        <v>776.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -50852,10 +50856,12 @@
     <row r="118" ht="24.75" customHeight="1" spans="1:9">
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
-      <c r="C118" s="74"/>
+      <c r="C118" s="74" t="s">
+        <v>139</v>
+      </c>
       <c r="D118" s="74"/>
       <c r="E118" s="87">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="F118" s="14"/>
       <c r="G118" s="14"/>
@@ -50918,7 +50924,7 @@
       <c r="A123" s="63"/>
       <c r="B123" s="64"/>
       <c r="C123" s="65" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D123" s="66"/>
       <c r="E123" s="37">
@@ -51101,7 +51107,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1154.02</v>
+        <v>809.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -51193,7 +51199,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>1154.02</v>
+        <v>809.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -51362,7 +51368,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -51465,7 +51471,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1739.02</v>
+        <v>1394.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -51557,7 +51563,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>1739.02</v>
+        <v>1394.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -51829,7 +51835,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>2755.02</v>
+        <v>2410.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -52362,7 +52368,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -52378,7 +52384,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6084.02</v>
+        <v>5739.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -52394,7 +52400,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6757.04</v>
+        <v>6068.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -54219,7 +54225,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>2755.02</v>
+        <v>2410.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -54388,7 +54394,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="73" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D129" s="74"/>
       <c r="E129" s="87">
@@ -54491,7 +54497,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3500.02</v>
+        <v>3155.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -54583,7 +54589,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>3500.02</v>
+        <v>3155.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -54752,7 +54758,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -54855,7 +54861,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5439.02</v>
+        <v>5094.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -54947,7 +54953,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>5439.02</v>
+        <v>5094.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -55116,7 +55122,7 @@
       <c r="A183" s="63"/>
       <c r="B183" s="64"/>
       <c r="C183" s="73" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D183" s="74"/>
       <c r="E183" s="87">
@@ -55219,7 +55225,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6084.02</v>
+        <v>5739.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -55749,7 +55755,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>673.02</v>
+        <v>328.98</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -55765,7 +55771,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>8701.02</v>
+        <v>8356.98</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -55781,7 +55787,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>9374.04</v>
+        <v>8685.96</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55880,7 +55886,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="101" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -57604,7 +57610,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>6084.02</v>
+        <v>5739.98</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -57876,7 +57882,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="89">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7100.02</v>
+        <v>6755.98</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -57968,7 +57974,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="89">
         <f ca="1">E136</f>
-        <v>7100.02</v>
+        <v>6755.98</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -58137,7 +58143,7 @@
       <c r="A156" s="63"/>
       <c r="B156" s="64"/>
       <c r="C156" s="73" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D156" s="74"/>
       <c r="E156" s="87">
@@ -58240,7 +58246,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="92">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>7685.02</v>
+        <v>7340.98</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -58332,7 +58338,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="92">
         <f ca="1">E163</f>
-        <v>7685.02</v>
+        <v>7340.98</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -58604,7 +58610,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="92">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>8701.02</v>
+        <v>8356.98</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>